<commit_message>
New rule + fixed project subsector/sector matching
</commit_message>
<xml_diff>
--- a/core/import_data/resources/cluster_project_mapping.xlsx
+++ b/core/import_data/resources/cluster_project_mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="121">
   <si>
     <t>ProjectCode</t>
   </si>
@@ -310,6 +310,75 @@
   </si>
   <si>
     <t>TRI/PHA/51/TAS/22</t>
+  </si>
+  <si>
+    <t>YEM/SOL/45/TAS/22</t>
+  </si>
+  <si>
+    <t>BAH/SOL/45/TAS/14</t>
+  </si>
+  <si>
+    <t>BDI/SOL/45/TAS/19</t>
+  </si>
+  <si>
+    <t>KAM/SOL/57/TAS/21</t>
+  </si>
+  <si>
+    <t>CRO/SOL/45/TAS/25</t>
+  </si>
+  <si>
+    <t>ETH/SOL/45/TAS/15</t>
+  </si>
+  <si>
+    <t>JAM/SOL/42/TAS/20</t>
+  </si>
+  <si>
+    <t>KEN/SOL/57/TAS/47</t>
+  </si>
+  <si>
+    <t>MOR/SOL/45/TAS/53</t>
+  </si>
+  <si>
+    <t>NEP/SOL/47/TAS/17</t>
+  </si>
+  <si>
+    <t>OMA/SOL/45/TAS/11</t>
+  </si>
+  <si>
+    <t>PAR/SOL/45/TAS/14</t>
+  </si>
+  <si>
+    <t>TUN/SOL/45/TAS/45</t>
+  </si>
+  <si>
+    <t>URU/SOL/45/TAS/43</t>
+  </si>
+  <si>
+    <t>VEN/SOL/45/TAS/103</t>
+  </si>
+  <si>
+    <t>ZIM/SOL/50/TAS/35</t>
+  </si>
+  <si>
+    <t>GLO/SEV/33/TAS/229</t>
+  </si>
+  <si>
+    <t>FUM</t>
+  </si>
+  <si>
+    <t>AFR/SEV/36/TAS/30</t>
+  </si>
+  <si>
+    <t>UGA/PHA/50/PRP/12</t>
+  </si>
+  <si>
+    <t>BHU/PHA/52/TAS/10</t>
+  </si>
+  <si>
+    <t>CPOP</t>
+  </si>
+  <si>
+    <t>ZIM/PHA/44/INV/29</t>
   </si>
 </sst>
 </file>
@@ -1595,108 +1664,194 @@
       <c r="C84" s="9"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
+      <c r="A85" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C85" s="9"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
+      <c r="A86" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C86" s="9"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
+      <c r="A87" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C87" s="9"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
+      <c r="A88" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C88" s="9"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
+      <c r="A89" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C89" s="9"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
+      <c r="A90" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C90" s="9"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
+      <c r="A91" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C91" s="9"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
+      <c r="A92" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C92" s="9"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
+      <c r="A93" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C93" s="9"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
+      <c r="A94" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C94" s="9"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
+      <c r="A95" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C95" s="9"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C96" s="9"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
+      <c r="A97" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C97" s="9"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
+      <c r="A98" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C98" s="9"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
+      <c r="A99" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C99" s="9"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
+      <c r="A100" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C100" s="9"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="9"/>
+      <c r="A101" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
+      <c r="A102" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="C102" s="9"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
+      <c r="A103" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="C103" s="9"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
+      <c r="A104" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="C104" s="9"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
+      <c r="A105" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="C105" s="9"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updated sector/subsector mapping for bp
</commit_message>
<xml_diff>
--- a/core/import_data/resources/cluster_project_mapping.xlsx
+++ b/core/import_data/resources/cluster_project_mapping.xlsx
@@ -6,19 +6,19 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1379</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1383</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="haB5BcTGuPiN/5DQvkzBjJrGDAlUoYzdxRZGwj0zLkg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BBsmOgaXbcSjtEhYoGBKpF0a0UL739VQ3W6ypvoDEqE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4035" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="1420">
   <si>
     <t>ProjectCode</t>
   </si>
@@ -4266,13 +4266,25 @@
   </si>
   <si>
     <t>ZIM/PHA/71/INV/47</t>
+  </si>
+  <si>
+    <t>GLO/SEV/26/TAS/170</t>
+  </si>
+  <si>
+    <t>GLO/SEV/30/TAS/208</t>
+  </si>
+  <si>
+    <t>GLO/SEV/32/TAS/223</t>
+  </si>
+  <si>
+    <t>GLO/SEV/45/TAS/263</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4294,6 +4306,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4303,7 +4320,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="hair">
@@ -4349,11 +4366,22 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4407,6 +4435,14 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -49930,10 +49966,140 @@
       <c r="X1379" s="5"/>
       <c r="Y1379" s="5"/>
     </row>
+    <row r="1380" ht="15.75" customHeight="1">
+      <c r="A1380" s="23" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1380" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1380" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1380" s="24"/>
+      <c r="E1380" s="24"/>
+      <c r="F1380" s="24"/>
+      <c r="G1380" s="24"/>
+      <c r="H1380" s="24"/>
+      <c r="I1380" s="24"/>
+      <c r="J1380" s="24"/>
+      <c r="K1380" s="25"/>
+      <c r="L1380" s="24"/>
+      <c r="M1380" s="24"/>
+      <c r="N1380" s="25"/>
+      <c r="O1380" s="24"/>
+      <c r="P1380" s="24"/>
+      <c r="Q1380" s="24"/>
+      <c r="R1380" s="24"/>
+      <c r="S1380" s="24"/>
+      <c r="T1380" s="5"/>
+      <c r="U1380" s="5"/>
+      <c r="V1380" s="5"/>
+      <c r="W1380" s="5"/>
+      <c r="X1380" s="5"/>
+      <c r="Y1380" s="5"/>
+    </row>
+    <row r="1381" ht="15.75" customHeight="1">
+      <c r="A1381" s="23" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1381" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1381" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1381" s="24"/>
+      <c r="E1381" s="24"/>
+      <c r="F1381" s="24"/>
+      <c r="G1381" s="24"/>
+      <c r="H1381" s="24"/>
+      <c r="I1381" s="24"/>
+      <c r="J1381" s="24"/>
+      <c r="K1381" s="25"/>
+      <c r="L1381" s="24"/>
+      <c r="M1381" s="24"/>
+      <c r="N1381" s="25"/>
+      <c r="O1381" s="24"/>
+      <c r="P1381" s="24"/>
+      <c r="Q1381" s="24"/>
+      <c r="R1381" s="24"/>
+      <c r="S1381" s="24"/>
+      <c r="T1381" s="5"/>
+      <c r="U1381" s="5"/>
+      <c r="V1381" s="5"/>
+      <c r="W1381" s="5"/>
+      <c r="X1381" s="5"/>
+      <c r="Y1381" s="5"/>
+    </row>
+    <row r="1382" ht="15.75" customHeight="1">
+      <c r="A1382" s="23" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1382" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1382" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1382" s="24"/>
+      <c r="E1382" s="24"/>
+      <c r="F1382" s="24"/>
+      <c r="G1382" s="24"/>
+      <c r="H1382" s="24"/>
+      <c r="I1382" s="24"/>
+      <c r="J1382" s="24"/>
+      <c r="K1382" s="25"/>
+      <c r="L1382" s="24"/>
+      <c r="M1382" s="24"/>
+      <c r="N1382" s="25"/>
+      <c r="O1382" s="24"/>
+      <c r="P1382" s="24"/>
+      <c r="Q1382" s="24"/>
+      <c r="R1382" s="24"/>
+      <c r="S1382" s="24"/>
+      <c r="T1382" s="5"/>
+      <c r="U1382" s="5"/>
+      <c r="V1382" s="5"/>
+      <c r="W1382" s="5"/>
+      <c r="X1382" s="5"/>
+      <c r="Y1382" s="5"/>
+    </row>
+    <row r="1383" ht="15.75" customHeight="1">
+      <c r="A1383" s="23" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B1383" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1383" s="26"/>
+      <c r="D1383" s="24"/>
+      <c r="E1383" s="24"/>
+      <c r="F1383" s="24"/>
+      <c r="G1383" s="24"/>
+      <c r="H1383" s="24"/>
+      <c r="I1383" s="24"/>
+      <c r="J1383" s="24"/>
+      <c r="K1383" s="25"/>
+      <c r="L1383" s="24"/>
+      <c r="M1383" s="24"/>
+      <c r="N1383" s="25"/>
+      <c r="O1383" s="24"/>
+      <c r="P1383" s="24"/>
+      <c r="Q1383" s="24"/>
+      <c r="R1383" s="24"/>
+      <c r="S1383" s="24"/>
+      <c r="T1383" s="5"/>
+      <c r="U1383" s="5"/>
+      <c r="V1383" s="5"/>
+      <c r="W1383" s="5"/>
+      <c r="X1383" s="5"/>
+      <c r="Y1383" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$D$1379">
-    <sortState ref="A1:D1379">
-      <sortCondition ref="A1:A1379"/>
+  <autoFilter ref="$A$1:$D$1383">
+    <sortState ref="A1:D1383">
+      <sortCondition ref="A1:A1383"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated sector/subsector mapping for bp (#160)
* Updated sector/subsector mapping for bp

* fixed tests

* Merge migration

* updated bp export
</commit_message>
<xml_diff>
--- a/core/import_data/resources/cluster_project_mapping.xlsx
+++ b/core/import_data/resources/cluster_project_mapping.xlsx
@@ -6,19 +6,19 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1379</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$D$1383</definedName>
   </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="haB5BcTGuPiN/5DQvkzBjJrGDAlUoYzdxRZGwj0zLkg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BBsmOgaXbcSjtEhYoGBKpF0a0UL739VQ3W6ypvoDEqE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4035" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="1420">
   <si>
     <t>ProjectCode</t>
   </si>
@@ -4266,13 +4266,25 @@
   </si>
   <si>
     <t>ZIM/PHA/71/INV/47</t>
+  </si>
+  <si>
+    <t>GLO/SEV/26/TAS/170</t>
+  </si>
+  <si>
+    <t>GLO/SEV/30/TAS/208</t>
+  </si>
+  <si>
+    <t>GLO/SEV/32/TAS/223</t>
+  </si>
+  <si>
+    <t>GLO/SEV/45/TAS/263</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4294,6 +4306,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4303,7 +4320,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="hair">
@@ -4349,11 +4366,22 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4407,6 +4435,14 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -49930,10 +49966,140 @@
       <c r="X1379" s="5"/>
       <c r="Y1379" s="5"/>
     </row>
+    <row r="1380" ht="15.75" customHeight="1">
+      <c r="A1380" s="23" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1380" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1380" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1380" s="24"/>
+      <c r="E1380" s="24"/>
+      <c r="F1380" s="24"/>
+      <c r="G1380" s="24"/>
+      <c r="H1380" s="24"/>
+      <c r="I1380" s="24"/>
+      <c r="J1380" s="24"/>
+      <c r="K1380" s="25"/>
+      <c r="L1380" s="24"/>
+      <c r="M1380" s="24"/>
+      <c r="N1380" s="25"/>
+      <c r="O1380" s="24"/>
+      <c r="P1380" s="24"/>
+      <c r="Q1380" s="24"/>
+      <c r="R1380" s="24"/>
+      <c r="S1380" s="24"/>
+      <c r="T1380" s="5"/>
+      <c r="U1380" s="5"/>
+      <c r="V1380" s="5"/>
+      <c r="W1380" s="5"/>
+      <c r="X1380" s="5"/>
+      <c r="Y1380" s="5"/>
+    </row>
+    <row r="1381" ht="15.75" customHeight="1">
+      <c r="A1381" s="23" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1381" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1381" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1381" s="24"/>
+      <c r="E1381" s="24"/>
+      <c r="F1381" s="24"/>
+      <c r="G1381" s="24"/>
+      <c r="H1381" s="24"/>
+      <c r="I1381" s="24"/>
+      <c r="J1381" s="24"/>
+      <c r="K1381" s="25"/>
+      <c r="L1381" s="24"/>
+      <c r="M1381" s="24"/>
+      <c r="N1381" s="25"/>
+      <c r="O1381" s="24"/>
+      <c r="P1381" s="24"/>
+      <c r="Q1381" s="24"/>
+      <c r="R1381" s="24"/>
+      <c r="S1381" s="24"/>
+      <c r="T1381" s="5"/>
+      <c r="U1381" s="5"/>
+      <c r="V1381" s="5"/>
+      <c r="W1381" s="5"/>
+      <c r="X1381" s="5"/>
+      <c r="Y1381" s="5"/>
+    </row>
+    <row r="1382" ht="15.75" customHeight="1">
+      <c r="A1382" s="23" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1382" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1382" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1382" s="24"/>
+      <c r="E1382" s="24"/>
+      <c r="F1382" s="24"/>
+      <c r="G1382" s="24"/>
+      <c r="H1382" s="24"/>
+      <c r="I1382" s="24"/>
+      <c r="J1382" s="24"/>
+      <c r="K1382" s="25"/>
+      <c r="L1382" s="24"/>
+      <c r="M1382" s="24"/>
+      <c r="N1382" s="25"/>
+      <c r="O1382" s="24"/>
+      <c r="P1382" s="24"/>
+      <c r="Q1382" s="24"/>
+      <c r="R1382" s="24"/>
+      <c r="S1382" s="24"/>
+      <c r="T1382" s="5"/>
+      <c r="U1382" s="5"/>
+      <c r="V1382" s="5"/>
+      <c r="W1382" s="5"/>
+      <c r="X1382" s="5"/>
+      <c r="Y1382" s="5"/>
+    </row>
+    <row r="1383" ht="15.75" customHeight="1">
+      <c r="A1383" s="23" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B1383" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1383" s="26"/>
+      <c r="D1383" s="24"/>
+      <c r="E1383" s="24"/>
+      <c r="F1383" s="24"/>
+      <c r="G1383" s="24"/>
+      <c r="H1383" s="24"/>
+      <c r="I1383" s="24"/>
+      <c r="J1383" s="24"/>
+      <c r="K1383" s="25"/>
+      <c r="L1383" s="24"/>
+      <c r="M1383" s="24"/>
+      <c r="N1383" s="25"/>
+      <c r="O1383" s="24"/>
+      <c r="P1383" s="24"/>
+      <c r="Q1383" s="24"/>
+      <c r="R1383" s="24"/>
+      <c r="S1383" s="24"/>
+      <c r="T1383" s="5"/>
+      <c r="U1383" s="5"/>
+      <c r="V1383" s="5"/>
+      <c r="W1383" s="5"/>
+      <c r="X1383" s="5"/>
+      <c r="Y1383" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$D$1379">
-    <sortState ref="A1:D1379">
-      <sortCondition ref="A1:A1379"/>
+  <autoFilter ref="$A$1:$D$1383">
+    <sortState ref="A1:D1383">
+      <sortCondition ref="A1:A1383"/>
     </sortState>
   </autoFilter>
   <drawing r:id="rId1"/>

</xml_diff>